<commit_message>
fixed some port data
</commit_message>
<xml_diff>
--- a/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/Tables22-28.xlsx
+++ b/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/Tables22-28.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/wc_cc_synthesis/data/landings/cdfw/public/fish_bulletins/raw/fb102/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4306C0-9ED5-D545-A5C7-B2A129236529}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59EB3A7A-A27F-5E40-BF68-835F171DF1BC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23180" yWindow="1140" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$407</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="149">
   <si>
     <t>•Spiny lobster</t>
   </si>
@@ -461,6 +464,12 @@
   </si>
   <si>
     <t>pounds</t>
+  </si>
+  <si>
+    <t>All species</t>
+  </si>
+  <si>
+    <t>All other species</t>
   </si>
 </sst>
 </file>
@@ -844,17 +853,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E407"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A262" workbookViewId="0">
+      <selection activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -879,8 +888,11 @@
       <c r="A2" s="1" t="s">
         <v>142</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>132</v>
+      </c>
       <c r="C2" s="1" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3">
         <v>2519140</v>
@@ -1723,7 +1735,7 @@
         <v>95</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="D53" s="3">
         <v>5990</v>
@@ -1755,15 +1767,22 @@
       <c r="C55" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="D55" s="5">
+        <v>0</v>
+      </c>
+      <c r="E55" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B56" s="1" t="s">
+        <v>144</v>
+      </c>
       <c r="C56" s="1" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="D56" s="6">
         <v>259478</v>
@@ -2134,8 +2153,12 @@
       <c r="C79" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
+      <c r="D79" s="5">
+        <v>0</v>
+      </c>
+      <c r="E79" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
@@ -2226,7 +2249,7 @@
         <v>95</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D85" s="3">
         <v>1324</v>
@@ -2270,10 +2293,10 @@
         <v>3</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>97</v>
+        <v>17</v>
       </c>
       <c r="D88" s="3">
         <v>14047187</v>
@@ -3325,7 +3348,7 @@
         <v>95</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="D152" s="3">
         <v>2326</v>
@@ -3355,18 +3378,22 @@
       <c r="C154" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D154" s="5"/>
-      <c r="E154" s="5"/>
+      <c r="D154" s="5">
+        <v>0</v>
+      </c>
+      <c r="E154" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>105</v>
+        <v>17</v>
       </c>
       <c r="D155" s="3">
         <v>1939001</v>
@@ -4017,7 +4044,7 @@
         <v>95</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="D194" s="3">
         <v>546</v>
@@ -4047,18 +4074,22 @@
       <c r="C196" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D196" s="5"/>
-      <c r="E196" s="5"/>
+      <c r="D196" s="5">
+        <v>0</v>
+      </c>
+      <c r="E196" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="D197" s="3">
         <v>1658638</v>
@@ -4769,8 +4800,12 @@
       <c r="C240" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D240" s="5"/>
-      <c r="E240" s="5"/>
+      <c r="D240" s="5">
+        <v>0</v>
+      </c>
+      <c r="E240" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
@@ -4810,8 +4845,12 @@
       <c r="C243" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D243" s="5"/>
-      <c r="E243" s="5"/>
+      <c r="D243" s="5">
+        <v>0</v>
+      </c>
+      <c r="E243" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
@@ -4821,7 +4860,7 @@
         <v>95</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="D244" s="3">
         <v>2291</v>
@@ -4851,18 +4890,22 @@
       <c r="C246" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D246" s="5"/>
-      <c r="E246" s="5"/>
+      <c r="D246" s="5">
+        <v>0</v>
+      </c>
+      <c r="E246" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>116</v>
+        <v>17</v>
       </c>
       <c r="D247" s="3">
         <v>40390320</v>
@@ -6794,7 +6837,7 @@
         <v>95</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>13</v>
+        <v>148</v>
       </c>
       <c r="D363" s="3">
         <v>3585</v>
@@ -6838,10 +6881,10 @@
         <v>7</v>
       </c>
       <c r="B366" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>127</v>
+        <v>17</v>
       </c>
       <c r="D366" s="3">
         <v>20714483</v>
@@ -7322,8 +7365,12 @@
       <c r="C395" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D395" s="5"/>
-      <c r="E395" s="5"/>
+      <c r="D395" s="5">
+        <v>0</v>
+      </c>
+      <c r="E395" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A396" s="1" t="s">
@@ -7478,7 +7525,7 @@
         <v>95</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>13</v>
+        <v>147</v>
       </c>
       <c r="D405" s="3">
         <v>1155</v>
@@ -7508,10 +7555,15 @@
       <c r="C407" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D407" s="5"/>
-      <c r="E407" s="5"/>
+      <c r="D407" s="5">
+        <v>0</v>
+      </c>
+      <c r="E407" s="5">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E407" xr:uid="{79CFA585-A3C8-7540-B182-A62E5C07FBD2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>